<commit_message>
Fase 3: Reportes PDF + Email + correcciones PDF
- Generación de PDFs por comprador usando fpdf2
- Envío de correos vía Microsoft Graph API (Azure AD)
- Orquestador de reportes con modos --report, --report-only, --email, --dry-run
- Template HTML Jinja2 para cuerpo de correo
- Agrupamiento por EMAIL del comprador (no por empresa)
- Filtrado de cursos con 0 estudiantes en PDFs
- Detección de Excel disfrazado de CSV en sence_reader
- Correcciones al scraper: reset búsqueda entre cursos
- 71 tests pasando + 1 skipped

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/config/compradores_tecnipro.xlsx
+++ b/data/config/compradores_tecnipro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyjva\Desktop\tecnipro-reportes\data\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5440FFB0-6FB8-4178-905D-B42939131AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD7137F-E3F7-42A0-B8F8-D83CF9A9CDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22276" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="50">
   <si>
     <t>ID Curso Moodle</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>jortizleiva@gmail.com</t>
+  </si>
+  <si>
+    <t>jortizleiva@duocapital.cl</t>
+  </si>
+  <si>
+    <t>ygonzalez@duocapital.cl</t>
   </si>
 </sst>
 </file>
@@ -588,7 +594,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -651,7 +657,7 @@
         <v>46</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -745,7 +751,7 @@
         <v>46</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -770,7 +776,7 @@
         <v>46</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -1014,7 +1020,7 @@
         <v>46</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -1039,7 +1045,7 @@
         <v>46</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -1064,7 +1070,7 @@
         <v>46</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -1089,7 +1095,7 @@
         <v>46</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -1167,7 +1173,9 @@
   <autoFilter ref="A1:I23" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{BEF163BC-1E57-441C-A2E5-14A8DCC6E5BF}"/>
-    <hyperlink ref="G3:G23" r:id="rId2" display="jortizleiva@gmail.com" xr:uid="{B40C3A4D-AD24-459F-B969-4D8BF6A72660}"/>
+    <hyperlink ref="G6:G7" r:id="rId2" display="jortizleiva@duocapital.cl" xr:uid="{C44CBD03-DC00-4224-8E79-1C6B4610672C}"/>
+    <hyperlink ref="G17:G19" r:id="rId3" display="jortizleiva@duocapital.cl" xr:uid="{E7F627FA-B65C-4F13-8A52-88BDE4E2CA39}"/>
+    <hyperlink ref="G20" r:id="rId4" xr:uid="{70C982C4-8CA0-4D83-88D9-3B43BFC3828C}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1322,6 +1330,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="23fd0960-4c5e-41b8-aaad-16165ded4b12">
@@ -1330,15 +1347,6 @@
     <TaxCatchAll xmlns="3df6dcc6-9dc0-41ca-ab5b-1924eab6674a" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1577,20 +1585,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61140A6C-E896-4F49-ABF8-C24F4076BB55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31AFD776-EBC8-4393-8E65-D25BE7DFAF9C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="23fd0960-4c5e-41b8-aaad-16165ded4b12"/>
     <ds:schemaRef ds:uri="3df6dcc6-9dc0-41ca-ab5b-1924eab6674a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61140A6C-E896-4F49-ABF8-C24F4076BB55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>